<commit_message>
Manual Mining Class Separation (Stable?)
</commit_message>
<xml_diff>
--- a/Chi-Test__b1(1 ).csv__b3(1 2 ).csv_.xlsx
+++ b/Chi-Test__b1(1 ).csv__b3(1 2 ).csv_.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="343">
   <si>
     <t>Probability(0.05/0.01/0.001)</t>
   </si>
@@ -1374,13 +1374,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE60"/>
+  <dimension ref="A1:O60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1450,56 +1450,8 @@
       <c r="O4" t="s">
         <v>19</v>
       </c>
-      <c r="P4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>13</v>
-      </c>
-      <c r="R4" t="s">
-        <v>14</v>
-      </c>
-      <c r="S4" t="s">
-        <v>15</v>
-      </c>
-      <c r="T4" t="s">
-        <v>16</v>
-      </c>
-      <c r="U4" t="s">
-        <v>17</v>
-      </c>
-      <c r="V4" t="s">
-        <v>18</v>
-      </c>
-      <c r="W4" t="s">
-        <v>19</v>
-      </c>
-      <c r="X4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>18</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31">
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1547,7 +1499,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1595,7 +1547,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1643,7 +1595,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1691,7 +1643,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -1739,7 +1691,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -1787,7 +1739,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -1835,7 +1787,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -1883,7 +1835,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -1931,7 +1883,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -1979,7 +1931,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>79</v>
       </c>
@@ -2027,7 +1979,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>85</v>
       </c>

</xml_diff>